<commit_message>
Ajuste para substituir o ponto por virgula, nas audiencias
</commit_message>
<xml_diff>
--- a/Resources/04_07_2019.xlsx
+++ b/Resources/04_07_2019.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="150" yWindow="615" windowWidth="23655" windowHeight="9150"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Plan1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Plan2" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Plan3" sheetId="3" r:id="rId5"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -102,23 +105,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,11 +131,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -144,69 +155,340 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="33.57"/>
-    <col customWidth="1" min="3" max="3" width="15.71"/>
-    <col customWidth="1" min="4" max="4" width="14.14"/>
-    <col customWidth="1" min="5" max="26" width="8.71"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -220,23 +502,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>0.2707986111111111</v>
+        <v>0.27079861111111109</v>
       </c>
       <c r="D2" s="5">
         <v>0.22913194444444443</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -245,12 +527,12 @@
         <v>0.22930555555555554</v>
       </c>
       <c r="D3" s="5">
-        <v>0.2499421296296296</v>
+        <v>0.24994212962962961</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -259,12 +541,12 @@
         <v>0.25</v>
       </c>
       <c r="D4" s="5">
-        <v>0.2916666666666667</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -276,23 +558,23 @@
         <v>0.33327546296296295</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D6" s="5">
         <v>0.4375</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -304,9 +586,9 @@
         <v>0.45515046296296297</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -315,12 +597,12 @@
         <v>0.45549768518518513</v>
       </c>
       <c r="D8" s="5">
-        <v>0.5004050925925926</v>
+        <v>0.50040509259259258</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -329,82 +611,82 @@
         <v>0.5005208333333333</v>
       </c>
       <c r="D9" s="5">
-        <v>0.5628472222222222</v>
+        <v>0.56284722222222217</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5">
-        <v>0.562974537037037</v>
+        <v>0.56297453703703704</v>
       </c>
       <c r="D10" s="5">
-        <v>0.6243055555555556</v>
+        <v>0.62430555555555556</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="5">
-        <v>0.6243055555555556</v>
+        <v>0.62430555555555556</v>
       </c>
       <c r="D11" s="5">
-        <v>0.6776388888888888</v>
+        <v>0.67763888888888879</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5">
-        <v>0.6776388888888888</v>
+        <v>0.67763888888888879</v>
       </c>
       <c r="D12" s="5">
-        <v>0.7301851851851852</v>
+        <v>0.73018518518518516</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5">
-        <v>0.7301851851851852</v>
+        <v>0.73018518518518516</v>
       </c>
       <c r="D13" s="5">
-        <v>0.7645833333333334</v>
+        <v>0.76458333333333339</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="5">
-        <v>0.7645833333333334</v>
+        <v>0.76458333333333339</v>
       </c>
       <c r="D14" s="5">
-        <v>0.8039699074074074</v>
+        <v>0.80396990740740737</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -413,124 +695,124 @@
         <v>0.8041666666666667</v>
       </c>
       <c r="D15" s="5">
-        <v>0.8213541666666666</v>
+        <v>0.82135416666666661</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="5">
-        <v>0.8215277777777777</v>
+        <v>0.82152777777777775</v>
       </c>
       <c r="D16" s="5">
-        <v>0.8541666666666666</v>
+        <v>0.85416666666666663</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75">
       <c r="A17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="5">
-        <v>0.8545138888888889</v>
+        <v>0.85451388888888891</v>
       </c>
       <c r="D17" s="5">
-        <v>0.8714699074074074</v>
+        <v>0.87146990740740737</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75">
       <c r="A18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="5">
-        <v>0.8719328703703703</v>
+        <v>0.87193287037037026</v>
       </c>
       <c r="D18" s="5">
-        <v>0.9127314814814814</v>
+        <v>0.91273148148148142</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="15.75">
       <c r="A19" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="5">
-        <v>0.9132523148148147</v>
+        <v>0.91325231481481473</v>
       </c>
       <c r="D19" s="5">
-        <v>0.9383101851851853</v>
+        <v>0.93831018518518527</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="15.75">
       <c r="A20" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="5">
-        <v>0.9383101851851853</v>
+        <v>0.93831018518518527</v>
       </c>
       <c r="D20" s="5">
-        <v>0.9825231481481481</v>
+        <v>0.98252314814814812</v>
       </c>
     </row>
-    <row r="21" ht="18.0" customHeight="1">
+    <row r="21" spans="1:26" ht="18" customHeight="1">
       <c r="A21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="5">
-        <v>0.9826967592592593</v>
+        <v>0.98269675925925926</v>
       </c>
       <c r="D21" s="5">
-        <v>0.048483796296296296</v>
+        <v>4.8483796296296296E-2</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="5">
-        <v>0.048483796296296296</v>
+        <v>4.8483796296296296E-2</v>
       </c>
       <c r="D22" s="5">
-        <v>0.0911111111111111</v>
+        <v>9.1111111111111101E-2</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="3">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="5">
-        <v>0.1609722222222222</v>
+        <v>0.16097222222222221</v>
       </c>
       <c r="D23" s="5">
         <v>0.11229166666666668</v>
       </c>
     </row>
-    <row r="24" ht="24.0" customHeight="1">
+    <row r="24" spans="1:26" ht="24" customHeight="1">
       <c r="A24" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>26</v>
@@ -539,7 +821,7 @@
         <v>0.11275462962962964</v>
       </c>
       <c r="D24" s="5">
-        <v>0.1396875</v>
+        <v>0.13968749999999999</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -564,9 +846,9 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>27</v>
@@ -575,57 +857,57 @@
         <v>0.13974537037037038</v>
       </c>
       <c r="D25" s="5">
-        <v>0.2501041666666667</v>
+        <v>0.25010416666666668</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5">
-        <v>0.4895833333333333</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="D26" s="5">
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
-        <v>0.4583333333333333</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D27" s="5">
-        <v>0.5833333333333334</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="3">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
-        <v>0.2916666666666667</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D28" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="3">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C29" s="5">
         <v>0.25</v>
@@ -634,26 +916,26 @@
         <v>0.24930555555555556</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5">
-        <v>0.2916666666666667</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D30" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C31" s="5">
         <v>0.5</v>
@@ -662,49 +944,49 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="C32" s="5">
         <v>0.75</v>
       </c>
       <c r="D32" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="3">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C33" s="5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D33" s="5">
         <v>0.24930555555555556</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -1658,24 +1940,20 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2659,24 +2937,20 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3660,9 +3934,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>